<commit_message>
Add run.param and helper script for experiments
</commit_message>
<xml_diff>
--- a/PD1_Candidates.xlsx
+++ b/PD1_Candidates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colby/PD1_Fab_Diffusion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B6DCD5-E5E1-D848-9B35-A03E8C8F762D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400CC35E-E35A-8142-BC54-D7F8BA4263CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20180" xr2:uid="{434B73E4-B198-41A3-8504-E0565A9D3A36}"/>
   </bookViews>
@@ -1202,10 +1202,10 @@
   <dimension ref="A1:AO43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2098,7 +2098,7 @@
       <c r="AN10" s="3"/>
       <c r="AO10" s="3"/>
     </row>
-    <row r="11" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
@@ -2179,7 +2179,7 @@
       <c r="AN11" s="3"/>
       <c r="AO11" s="3"/>
     </row>
-    <row r="12" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -2260,7 +2260,7 @@
       <c r="AN12" s="3"/>
       <c r="AO12" s="3"/>
     </row>
-    <row r="13" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -2341,7 +2341,7 @@
       <c r="AN13" s="3"/>
       <c r="AO13" s="3"/>
     </row>
-    <row r="14" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
@@ -2422,7 +2422,7 @@
       <c r="AN14" s="3"/>
       <c r="AO14" s="3"/>
     </row>
-    <row r="15" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
@@ -2503,7 +2503,7 @@
       <c r="AN15" s="3"/>
       <c r="AO15" s="3"/>
     </row>
-    <row r="16" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
@@ -2584,7 +2584,7 @@
       <c r="AN16" s="3"/>
       <c r="AO16" s="3"/>
     </row>
-    <row r="17" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
@@ -2665,7 +2665,7 @@
       <c r="AN17" s="3"/>
       <c r="AO17" s="3"/>
     </row>
-    <row r="18" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="AN18" s="3"/>
       <c r="AO18" s="3"/>
     </row>
-    <row r="19" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
@@ -2908,7 +2908,7 @@
       <c r="AN20" s="3"/>
       <c r="AO20" s="3"/>
     </row>
-    <row r="21" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -2989,7 +2989,7 @@
       <c r="AN21" s="3"/>
       <c r="AO21" s="3"/>
     </row>
-    <row r="22" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>34</v>
       </c>
@@ -3232,7 +3232,7 @@
       <c r="AN24" s="3"/>
       <c r="AO24" s="3"/>
     </row>
-    <row r="25" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>37</v>
       </c>
@@ -3313,7 +3313,7 @@
       <c r="AN25" s="3"/>
       <c r="AO25" s="3"/>
     </row>
-    <row r="26" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
@@ -3475,7 +3475,7 @@
       <c r="AN27" s="3"/>
       <c r="AO27" s="3"/>
     </row>
-    <row r="28" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>40</v>
       </c>
@@ -3556,7 +3556,7 @@
       <c r="AN28" s="3"/>
       <c r="AO28" s="3"/>
     </row>
-    <row r="29" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>41</v>
       </c>
@@ -3637,7 +3637,7 @@
       <c r="AN29" s="3"/>
       <c r="AO29" s="3"/>
     </row>
-    <row r="30" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>42</v>
       </c>
@@ -3718,7 +3718,7 @@
       <c r="AN30" s="3"/>
       <c r="AO30" s="3"/>
     </row>
-    <row r="31" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>43</v>
       </c>
@@ -3799,7 +3799,7 @@
       <c r="AN31" s="3"/>
       <c r="AO31" s="3"/>
     </row>
-    <row r="32" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>44</v>
       </c>
@@ -3880,7 +3880,7 @@
       <c r="AN32" s="3"/>
       <c r="AO32" s="3"/>
     </row>
-    <row r="33" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>45</v>
       </c>
@@ -3961,7 +3961,7 @@
       <c r="AN33" s="3"/>
       <c r="AO33" s="3"/>
     </row>
-    <row r="34" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>46</v>
       </c>
@@ -4042,7 +4042,7 @@
       <c r="AN34" s="3"/>
       <c r="AO34" s="3"/>
     </row>
-    <row r="35" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -4123,7 +4123,7 @@
       <c r="AN35" s="3"/>
       <c r="AO35" s="3"/>
     </row>
-    <row r="36" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>48</v>
       </c>
@@ -4285,7 +4285,7 @@
       <c r="AN37" s="3"/>
       <c r="AO37" s="3"/>
     </row>
-    <row r="38" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>50</v>
       </c>
@@ -4366,7 +4366,7 @@
       <c r="AN38" s="3"/>
       <c r="AO38" s="3"/>
     </row>
-    <row r="39" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>51</v>
       </c>
@@ -4528,7 +4528,7 @@
       <c r="AN40" s="3"/>
       <c r="AO40" s="3"/>
     </row>
-    <row r="41" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>53</v>
       </c>
@@ -4690,7 +4690,7 @@
       <c r="AN42" s="3"/>
       <c r="AO42" s="3"/>
     </row>
-    <row r="43" spans="1:41" ht="80" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:41" ht="64" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>55</v>
       </c>

</xml_diff>